<commit_message>
Updated Excel reports with test case results
</commit_message>
<xml_diff>
--- a/NopCommerce/Test_Suites/TC_SignupTest_Report.xlsx
+++ b/NopCommerce/Test_Suites/TC_SignupTest_Report.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT_Projects\NopCommerce\Test_Suites\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -22,6 +27,12 @@
     <t>Description</t>
   </si>
   <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
     <t>Email</t>
   </si>
   <si>
@@ -43,6 +54,21 @@
     <t>TC_01</t>
   </si>
   <si>
+    <t>Valid Sign up using minimum required data</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Dummy</t>
+  </si>
+  <si>
+    <t>CorrectEmail@gmail.com</t>
+  </si>
+  <si>
+    <t>thatshouldmakeit</t>
+  </si>
+  <si>
     <t>TC_02</t>
   </si>
   <si>
@@ -50,13 +76,16 @@
   </si>
   <si>
     <t>TC_04</t>
+  </si>
+  <si>
+    <t>Registration Successful and redirected to Login Page</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,6 +118,12 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Inherit"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -139,7 +174,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -158,6 +193,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -464,25 +505,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H5"/>
+      <selection activeCell="H2" sqref="H2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.140625" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" customWidth="1"/>
-    <col min="5" max="5" width="33" customWidth="1"/>
-    <col min="6" max="6" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" customWidth="1"/>
-    <col min="8" max="8" width="61" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="8" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+    <col min="7" max="7" width="33" customWidth="1"/>
+    <col min="8" max="8" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" customWidth="1"/>
+    <col min="10" max="10" width="61" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17.25" thickBot="1">
+    <row r="1" spans="1:10" ht="17.25" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -507,59 +550,89 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" ht="17.25" thickBot="1">
+    <row r="2" spans="1:10" ht="33.75" customHeight="1" thickBot="1">
       <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
     </row>
-    <row r="3" spans="1:8" ht="17.25" thickBot="1">
+    <row r="3" spans="1:10" ht="17.25" customHeight="1" thickBot="1">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="3"/>
+      <c r="C3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="5"/>
+      <c r="E3" s="3"/>
       <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
     </row>
-    <row r="4" spans="1:8" ht="17.25" thickBot="1">
+    <row r="4" spans="1:10" ht="17.25" customHeight="1" thickBot="1">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
+      <c r="C4" s="4"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="5"/>
+      <c r="E4" s="3"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
     </row>
-    <row r="5" spans="1:8" ht="17.25" thickBot="1">
+    <row r="5" spans="1:10" ht="17.25" customHeight="1" thickBot="1">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="5"/>
+      <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
     </row>
-    <row r="15" spans="1:8">
-      <c r="E15" s="6"/>
+    <row r="15" spans="1:10">
+      <c r="G15" s="6"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>